<commit_message>
Fix imports and record format
</commit_message>
<xml_diff>
--- a/user_data.xlsx
+++ b/user_data.xlsx
@@ -1,24 +1,24 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11012"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10111"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dacort/src/athena-excel/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dcortesi/src/athena-excel/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{5840F0A7-BB51-DF4F-A643-EE8CBBD0F1FD}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3ADC36B9-8C15-9043-A0D9-3901E5242E9B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2780" yWindow="1500" windowWidth="28040" windowHeight="17440" activeTab="1" xr2:uid="{6BC5648E-3119-704D-AEA2-41DD9BFD63E7}"/>
+    <workbookView xWindow="2780" yWindow="1500" windowWidth="28040" windowHeight="17440" xr2:uid="{6BC5648E-3119-704D-AEA2-41DD9BFD63E7}"/>
   </bookViews>
   <sheets>
-    <sheet name="Logs" sheetId="2" r:id="rId1"/>
-    <sheet name="Users" sheetId="1" r:id="rId2"/>
+    <sheet name="logs" sheetId="2" r:id="rId1"/>
+    <sheet name="users" sheetId="1" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="sheet1" localSheetId="1">Users!$A$1:$E$4</definedName>
-    <definedName name="sheet2" localSheetId="0">Logs!$A$1:$F$82</definedName>
+    <definedName name="sheet1" localSheetId="1">users!$A$1:$E$4</definedName>
+    <definedName name="sheet2" localSheetId="0">logs!$A$1:$F$82</definedName>
   </definedNames>
   <calcPr calcId="181029"/>
   <extLst>
@@ -32,7 +32,7 @@
 <file path=xl/connections.xml><?xml version="1.0" encoding="utf-8"?>
 <connections xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16">
   <connection id="1" xr16:uid="{E9AA125B-5663-304D-9D3B-201D9EAC62BC}" name="sheet1" type="6" refreshedVersion="6" background="1" saveData="1">
-    <textPr codePage="10000" sourceFile="/Users/dacort/src/athena-excel/sheet1.csv" tab="0" comma="1">
+    <textPr sourceFile="/Users/dacort/src/athena-excel/sheet1.csv" tab="0" comma="1">
       <textFields count="5">
         <textField/>
         <textField/>
@@ -43,7 +43,7 @@
     </textPr>
   </connection>
   <connection id="2" xr16:uid="{807C4360-A8A5-774A-A3FC-41BF2CCA6683}" name="sheet2" type="6" refreshedVersion="6" background="1" saveData="1">
-    <textPr codePage="10000" sourceFile="/Users/dacort/src/athena-excel/sheet2.csv" tab="0" comma="1">
+    <textPr sourceFile="/Users/dacort/src/athena-excel/sheet2.csv" tab="0" comma="1">
       <textFields count="6">
         <textField/>
         <textField/>
@@ -1235,7 +1235,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{197EDE21-8D46-2A46-A9AF-85B146BDB8B7}">
   <dimension ref="A1:F82"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
@@ -2896,7 +2896,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{342E4032-87F5-7547-8B01-10F2A4823327}">
   <dimension ref="A1:E4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>

</xml_diff>